<commit_message>
bug correction in PeakValley
</commit_message>
<xml_diff>
--- a/data/Test_metodi_2.xlsx
+++ b/data/Test_metodi_2.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="540" windowWidth="25360" windowHeight="15380" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" firstSheet="2" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="Wisperx_RainNoDelta" sheetId="5" r:id="rId5"/>
     <sheet name="Wisperx_RainRangeDelta" sheetId="6" r:id="rId6"/>
     <sheet name="Wisperx_RainMidDelta" sheetId="7" r:id="rId7"/>
-    <sheet name="Wisperx_PeakValleyNoRange1" sheetId="9" r:id="rId8"/>
-    <sheet name="Wisperx_SimpleRangeNoRange" sheetId="11" r:id="rId9"/>
+    <sheet name="Wisperx_SimpleRangeNoRange" sheetId="8" r:id="rId8"/>
+    <sheet name="Wisperx_PeakValleyNoRange" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -4321,902 +4321,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F44"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>63</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D2">
-        <v>72.680999999999997</v>
-      </c>
-      <c r="E2">
-        <v>9.6809999999999974</v>
-      </c>
-      <c r="F2">
-        <v>0.13319849754406241</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>51</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D3">
-        <v>66.680999999999997</v>
-      </c>
-      <c r="E3">
-        <v>15.680999999999999</v>
-      </c>
-      <c r="F3">
-        <v>0.2351644396454762</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>50</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D4">
-        <v>66.180999999999997</v>
-      </c>
-      <c r="E4">
-        <v>16.181000000000001</v>
-      </c>
-      <c r="F4">
-        <v>0.2444961544854263</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>48</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D5">
-        <v>65.180999999999997</v>
-      </c>
-      <c r="E5">
-        <v>17.181000000000001</v>
-      </c>
-      <c r="F5">
-        <v>0.26358908270815112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>47</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D6">
-        <v>64.680999999999997</v>
-      </c>
-      <c r="E6">
-        <v>17.681000000000001</v>
-      </c>
-      <c r="F6">
-        <v>0.2733569363491597</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>46</v>
-      </c>
-      <c r="B7">
-        <v>4</v>
-      </c>
-      <c r="C7">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D7">
-        <v>64.180999999999997</v>
-      </c>
-      <c r="E7">
-        <v>18.181000000000001</v>
-      </c>
-      <c r="F7">
-        <v>0.28327698228447667</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>45</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D8">
-        <v>63.680999999999997</v>
-      </c>
-      <c r="E8">
-        <v>18.681000000000001</v>
-      </c>
-      <c r="F8">
-        <v>0.29335280538936259</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>44</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D9">
-        <v>63.180999999999997</v>
-      </c>
-      <c r="E9">
-        <v>19.181000000000001</v>
-      </c>
-      <c r="F9">
-        <v>0.30358810401861308</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>43</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D10">
-        <v>62.680999999999997</v>
-      </c>
-      <c r="E10">
-        <v>19.681000000000001</v>
-      </c>
-      <c r="F10">
-        <v>0.31398669453263339</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>42</v>
-      </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D11">
-        <v>62.180999999999997</v>
-      </c>
-      <c r="E11">
-        <v>20.181000000000001</v>
-      </c>
-      <c r="F11">
-        <v>0.32455251604187768</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>41</v>
-      </c>
-      <c r="B12">
-        <v>3</v>
-      </c>
-      <c r="C12">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D12">
-        <v>61.680999999999997</v>
-      </c>
-      <c r="E12">
-        <v>20.681000000000001</v>
-      </c>
-      <c r="F12">
-        <v>0.33528963538204631</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>38</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D13">
-        <v>60.180999999999997</v>
-      </c>
-      <c r="E13">
-        <v>22.181000000000001</v>
-      </c>
-      <c r="F13">
-        <v>0.36857147604725737</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>37</v>
-      </c>
-      <c r="B14">
-        <v>3.5</v>
-      </c>
-      <c r="C14">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D14">
-        <v>59.680999999999997</v>
-      </c>
-      <c r="E14">
-        <v>22.681000000000001</v>
-      </c>
-      <c r="F14">
-        <v>0.38003719776813388</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>36</v>
-      </c>
-      <c r="B15">
-        <v>70.5</v>
-      </c>
-      <c r="C15">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D15">
-        <v>59.180999999999997</v>
-      </c>
-      <c r="E15">
-        <v>23.181000000000001</v>
-      </c>
-      <c r="F15">
-        <v>0.39169665940082121</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>35</v>
-      </c>
-      <c r="B16">
-        <v>5</v>
-      </c>
-      <c r="C16">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D16">
-        <v>58.680999999999997</v>
-      </c>
-      <c r="E16">
-        <v>23.681000000000001</v>
-      </c>
-      <c r="F16">
-        <v>0.40355481331265652</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>34</v>
-      </c>
-      <c r="B17">
-        <v>43</v>
-      </c>
-      <c r="C17">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D17">
-        <v>58.180999999999997</v>
-      </c>
-      <c r="E17">
-        <v>24.181000000000001</v>
-      </c>
-      <c r="F17">
-        <v>0.4156167821109984</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>33</v>
-      </c>
-      <c r="B18">
-        <v>13</v>
-      </c>
-      <c r="C18">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D18">
-        <v>57.680999999999997</v>
-      </c>
-      <c r="E18">
-        <v>24.681000000000001</v>
-      </c>
-      <c r="F18">
-        <v>0.42788786602174023</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>32</v>
-      </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D19">
-        <v>57.180999999999997</v>
-      </c>
-      <c r="E19">
-        <v>25.181000000000001</v>
-      </c>
-      <c r="F19">
-        <v>0.44037355065493777</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>31</v>
-      </c>
-      <c r="B20">
-        <v>807</v>
-      </c>
-      <c r="C20">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D20">
-        <v>56.680999999999997</v>
-      </c>
-      <c r="E20">
-        <v>25.681000000000001</v>
-      </c>
-      <c r="F20">
-        <v>0.45307951518145412</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>30</v>
-      </c>
-      <c r="B21">
-        <v>527</v>
-      </c>
-      <c r="C21">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D21">
-        <v>56.180999999999997</v>
-      </c>
-      <c r="E21">
-        <v>26.181000000000001</v>
-      </c>
-      <c r="F21">
-        <v>0.46601164094622732</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>29</v>
-      </c>
-      <c r="B22">
-        <v>20</v>
-      </c>
-      <c r="C22">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D22">
-        <v>55.680999999999997</v>
-      </c>
-      <c r="E22">
-        <v>26.681000000000001</v>
-      </c>
-      <c r="F22">
-        <v>0.47917602054560798</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>28</v>
-      </c>
-      <c r="B23">
-        <v>223</v>
-      </c>
-      <c r="C23">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D23">
-        <v>55.180999999999997</v>
-      </c>
-      <c r="E23">
-        <v>27.181000000000001</v>
-      </c>
-      <c r="F23">
-        <v>0.49257896739819862</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>27</v>
-      </c>
-      <c r="B24">
-        <v>129</v>
-      </c>
-      <c r="C24">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D24">
-        <v>54.680999999999997</v>
-      </c>
-      <c r="E24">
-        <v>27.681000000000001</v>
-      </c>
-      <c r="F24">
-        <v>0.5062270258407856</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>26</v>
-      </c>
-      <c r="B25">
-        <v>452</v>
-      </c>
-      <c r="C25">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D25">
-        <v>54.180999999999997</v>
-      </c>
-      <c r="E25">
-        <v>28.181000000000001</v>
-      </c>
-      <c r="F25">
-        <v>0.52012698178328198</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>25</v>
-      </c>
-      <c r="B26">
-        <v>64</v>
-      </c>
-      <c r="C26">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D26">
-        <v>53.680999999999997</v>
-      </c>
-      <c r="E26">
-        <v>28.681000000000001</v>
-      </c>
-      <c r="F26">
-        <v>0.53428587395912885</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>24</v>
-      </c>
-      <c r="B27">
-        <v>1633</v>
-      </c>
-      <c r="C27">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D27">
-        <v>53.180999999999997</v>
-      </c>
-      <c r="E27">
-        <v>29.181000000000001</v>
-      </c>
-      <c r="F27">
-        <v>0.54871100581034582</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>23</v>
-      </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D28">
-        <v>52.680999999999997</v>
-      </c>
-      <c r="E28">
-        <v>29.681000000000001</v>
-      </c>
-      <c r="F28">
-        <v>0.56340995804939165</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>22</v>
-      </c>
-      <c r="B29">
-        <v>86</v>
-      </c>
-      <c r="C29">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D29">
-        <v>52.180999999999997</v>
-      </c>
-      <c r="E29">
-        <v>30.181000000000001</v>
-      </c>
-      <c r="F29">
-        <v>0.57839060194323599</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>21</v>
-      </c>
-      <c r="B30">
-        <v>216</v>
-      </c>
-      <c r="C30">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D30">
-        <v>51.680999999999997</v>
-      </c>
-      <c r="E30">
-        <v>30.681000000000001</v>
-      </c>
-      <c r="F30">
-        <v>0.59366111336854932</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>20</v>
-      </c>
-      <c r="B31">
-        <v>692</v>
-      </c>
-      <c r="C31">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D31">
-        <v>51.180999999999997</v>
-      </c>
-      <c r="E31">
-        <v>31.181000000000001</v>
-      </c>
-      <c r="F31">
-        <v>0.60922998769074455</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>18</v>
-      </c>
-      <c r="B32">
-        <v>3000</v>
-      </c>
-      <c r="C32">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D32">
-        <v>50.180999999999997</v>
-      </c>
-      <c r="E32">
-        <v>32.180999999999997</v>
-      </c>
-      <c r="F32">
-        <v>0.64129849943205597</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>17</v>
-      </c>
-      <c r="B33">
-        <v>1474</v>
-      </c>
-      <c r="C33">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D33">
-        <v>49.680999999999997</v>
-      </c>
-      <c r="E33">
-        <v>32.680999999999997</v>
-      </c>
-      <c r="F33">
-        <v>0.65781687164107006</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>16</v>
-      </c>
-      <c r="B34">
-        <v>22</v>
-      </c>
-      <c r="C34">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D34">
-        <v>49.180999999999997</v>
-      </c>
-      <c r="E34">
-        <v>33.180999999999997</v>
-      </c>
-      <c r="F34">
-        <v>0.67467111282812464</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A35">
-        <v>15</v>
-      </c>
-      <c r="B35">
-        <v>9</v>
-      </c>
-      <c r="C35">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D35">
-        <v>48.680999999999997</v>
-      </c>
-      <c r="E35">
-        <v>33.680999999999997</v>
-      </c>
-      <c r="F35">
-        <v>0.69187157207123928</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>14</v>
-      </c>
-      <c r="B36">
-        <v>57</v>
-      </c>
-      <c r="C36">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D36">
-        <v>48.180999999999997</v>
-      </c>
-      <c r="E36">
-        <v>34.180999999999997</v>
-      </c>
-      <c r="F36">
-        <v>0.70942902804009877</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>13</v>
-      </c>
-      <c r="B37">
-        <v>5</v>
-      </c>
-      <c r="C37">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D37">
-        <v>47.680999999999997</v>
-      </c>
-      <c r="E37">
-        <v>34.680999999999997</v>
-      </c>
-      <c r="F37">
-        <v>0.72735471152031206</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>12</v>
-      </c>
-      <c r="B38">
-        <v>1890</v>
-      </c>
-      <c r="C38">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D38">
-        <v>47.180999999999997</v>
-      </c>
-      <c r="E38">
-        <v>35.180999999999997</v>
-      </c>
-      <c r="F38">
-        <v>0.74566032936987348</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>11</v>
-      </c>
-      <c r="B39">
-        <v>13</v>
-      </c>
-      <c r="C39">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D39">
-        <v>46.680999999999997</v>
-      </c>
-      <c r="E39">
-        <v>35.680999999999997</v>
-      </c>
-      <c r="F39">
-        <v>0.7643580900152096</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>10</v>
-      </c>
-      <c r="B40">
-        <v>132</v>
-      </c>
-      <c r="C40">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D40">
-        <v>46.180999999999997</v>
-      </c>
-      <c r="E40">
-        <v>36.180999999999997</v>
-      </c>
-      <c r="F40">
-        <v>0.78346073060349497</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>9</v>
-      </c>
-      <c r="B41">
-        <v>318</v>
-      </c>
-      <c r="C41">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D41">
-        <v>45.680999999999997</v>
-      </c>
-      <c r="E41">
-        <v>36.680999999999997</v>
-      </c>
-      <c r="F41">
-        <v>0.8029815459381362</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>8</v>
-      </c>
-      <c r="B42">
-        <v>871</v>
-      </c>
-      <c r="C42">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D42">
-        <v>45.180999999999997</v>
-      </c>
-      <c r="E42">
-        <v>37.180999999999997</v>
-      </c>
-      <c r="F42">
-        <v>0.82293441933556144</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>7</v>
-      </c>
-      <c r="B43">
-        <v>2</v>
-      </c>
-      <c r="C43">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D43">
-        <v>44.680999999999997</v>
-      </c>
-      <c r="E43">
-        <v>37.680999999999997</v>
-      </c>
-      <c r="F43">
-        <v>0.84333385555381479</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>6</v>
-      </c>
-      <c r="B44">
-        <v>4</v>
-      </c>
-      <c r="C44">
-        <v>41.180999999999997</v>
-      </c>
-      <c r="D44">
-        <v>44.180999999999997</v>
-      </c>
-      <c r="E44">
-        <v>38.180999999999997</v>
-      </c>
-      <c r="F44">
-        <v>0.86419501595708559</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H135"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -7929,4 +7036,937 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>63</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>32.5</v>
+      </c>
+      <c r="D2">
+        <v>64</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1.5625E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>51</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>32.5</v>
+      </c>
+      <c r="D3">
+        <v>58</v>
+      </c>
+      <c r="E3">
+        <v>7</v>
+      </c>
+      <c r="F3">
+        <v>0.1206896551724138</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>57</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>0.1228070175438596</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>48</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>33</v>
+      </c>
+      <c r="D5">
+        <v>57</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>0.15789473684210531</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>47</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>33.5</v>
+      </c>
+      <c r="D6">
+        <v>57</v>
+      </c>
+      <c r="E6">
+        <v>10</v>
+      </c>
+      <c r="F6">
+        <v>0.17543859649122809</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>46</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>57</v>
+      </c>
+      <c r="E7">
+        <v>11</v>
+      </c>
+      <c r="F7">
+        <v>0.19298245614035089</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>45</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>34.5</v>
+      </c>
+      <c r="D8">
+        <v>57</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>0.2105263157894737</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>44</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>35</v>
+      </c>
+      <c r="D9">
+        <v>57</v>
+      </c>
+      <c r="E9">
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>0.22807017543859651</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>35.5</v>
+      </c>
+      <c r="D10">
+        <v>57</v>
+      </c>
+      <c r="E10">
+        <v>14</v>
+      </c>
+      <c r="F10">
+        <v>0.24561403508771931</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>42</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>36</v>
+      </c>
+      <c r="D11">
+        <v>57</v>
+      </c>
+      <c r="E11">
+        <v>15</v>
+      </c>
+      <c r="F11">
+        <v>0.26315789473684209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>41</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>36.5</v>
+      </c>
+      <c r="D12">
+        <v>57</v>
+      </c>
+      <c r="E12">
+        <v>16</v>
+      </c>
+      <c r="F12">
+        <v>0.2807017543859649</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>38</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>38</v>
+      </c>
+      <c r="D13">
+        <v>57</v>
+      </c>
+      <c r="E13">
+        <v>19</v>
+      </c>
+      <c r="F13">
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>37</v>
+      </c>
+      <c r="B14">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>38.5</v>
+      </c>
+      <c r="D14">
+        <v>57</v>
+      </c>
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>0.35087719298245612</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>37</v>
+      </c>
+      <c r="B15">
+        <v>1.5</v>
+      </c>
+      <c r="C15">
+        <v>18.5</v>
+      </c>
+      <c r="D15">
+        <v>37</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>36</v>
+      </c>
+      <c r="B16">
+        <v>52</v>
+      </c>
+      <c r="C16">
+        <v>39</v>
+      </c>
+      <c r="D16">
+        <v>57</v>
+      </c>
+      <c r="E16">
+        <v>21</v>
+      </c>
+      <c r="F16">
+        <v>0.36842105263157893</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>18.5</v>
+      </c>
+      <c r="C17">
+        <v>18</v>
+      </c>
+      <c r="D17">
+        <v>36</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>35</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18">
+        <v>39.5</v>
+      </c>
+      <c r="D18">
+        <v>57</v>
+      </c>
+      <c r="E18">
+        <v>22</v>
+      </c>
+      <c r="F18">
+        <v>0.38596491228070168</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>34</v>
+      </c>
+      <c r="B19">
+        <v>43</v>
+      </c>
+      <c r="C19">
+        <v>40</v>
+      </c>
+      <c r="D19">
+        <v>57</v>
+      </c>
+      <c r="E19">
+        <v>23</v>
+      </c>
+      <c r="F19">
+        <v>0.40350877192982448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>33</v>
+      </c>
+      <c r="B20">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>40.5</v>
+      </c>
+      <c r="D20">
+        <v>57</v>
+      </c>
+      <c r="E20">
+        <v>24</v>
+      </c>
+      <c r="F20">
+        <v>0.42105263157894729</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>32</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>41</v>
+      </c>
+      <c r="D21">
+        <v>57</v>
+      </c>
+      <c r="E21">
+        <v>25</v>
+      </c>
+      <c r="F21">
+        <v>0.43859649122807021</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>807</v>
+      </c>
+      <c r="C22">
+        <v>41.5</v>
+      </c>
+      <c r="D22">
+        <v>57</v>
+      </c>
+      <c r="E22">
+        <v>26</v>
+      </c>
+      <c r="F22">
+        <v>0.45614035087719301</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>527</v>
+      </c>
+      <c r="C23">
+        <v>41</v>
+      </c>
+      <c r="D23">
+        <v>56</v>
+      </c>
+      <c r="E23">
+        <v>26</v>
+      </c>
+      <c r="F23">
+        <v>0.4642857142857143</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>29</v>
+      </c>
+      <c r="B24">
+        <v>20</v>
+      </c>
+      <c r="C24">
+        <v>41.5</v>
+      </c>
+      <c r="D24">
+        <v>56</v>
+      </c>
+      <c r="E24">
+        <v>27</v>
+      </c>
+      <c r="F24">
+        <v>0.48214285714285721</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>223</v>
+      </c>
+      <c r="C25">
+        <v>41</v>
+      </c>
+      <c r="D25">
+        <v>55</v>
+      </c>
+      <c r="E25">
+        <v>27</v>
+      </c>
+      <c r="F25">
+        <v>0.49090909090909091</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>27</v>
+      </c>
+      <c r="B26">
+        <v>129</v>
+      </c>
+      <c r="C26">
+        <v>41.5</v>
+      </c>
+      <c r="D26">
+        <v>55</v>
+      </c>
+      <c r="E26">
+        <v>28</v>
+      </c>
+      <c r="F26">
+        <v>0.50909090909090904</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>452</v>
+      </c>
+      <c r="C27">
+        <v>42</v>
+      </c>
+      <c r="D27">
+        <v>55</v>
+      </c>
+      <c r="E27">
+        <v>29</v>
+      </c>
+      <c r="F27">
+        <v>0.52727272727272723</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>64</v>
+      </c>
+      <c r="C28">
+        <v>41.5</v>
+      </c>
+      <c r="D28">
+        <v>54</v>
+      </c>
+      <c r="E28">
+        <v>29</v>
+      </c>
+      <c r="F28">
+        <v>0.53703703703703709</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>1633</v>
+      </c>
+      <c r="C29">
+        <v>41</v>
+      </c>
+      <c r="D29">
+        <v>53</v>
+      </c>
+      <c r="E29">
+        <v>29</v>
+      </c>
+      <c r="F29">
+        <v>0.54716981132075471</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>23</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>40.5</v>
+      </c>
+      <c r="D30">
+        <v>52</v>
+      </c>
+      <c r="E30">
+        <v>29</v>
+      </c>
+      <c r="F30">
+        <v>0.55769230769230771</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>22</v>
+      </c>
+      <c r="B31">
+        <v>86</v>
+      </c>
+      <c r="C31">
+        <v>41</v>
+      </c>
+      <c r="D31">
+        <v>52</v>
+      </c>
+      <c r="E31">
+        <v>30</v>
+      </c>
+      <c r="F31">
+        <v>0.57692307692307687</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>21</v>
+      </c>
+      <c r="B32">
+        <v>216</v>
+      </c>
+      <c r="C32">
+        <v>41.5</v>
+      </c>
+      <c r="D32">
+        <v>52</v>
+      </c>
+      <c r="E32">
+        <v>31</v>
+      </c>
+      <c r="F32">
+        <v>0.59615384615384615</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>20</v>
+      </c>
+      <c r="B33">
+        <v>692</v>
+      </c>
+      <c r="C33">
+        <v>41</v>
+      </c>
+      <c r="D33">
+        <v>51</v>
+      </c>
+      <c r="E33">
+        <v>31</v>
+      </c>
+      <c r="F33">
+        <v>0.60784313725490191</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>18</v>
+      </c>
+      <c r="B34">
+        <v>3000</v>
+      </c>
+      <c r="C34">
+        <v>42</v>
+      </c>
+      <c r="D34">
+        <v>51</v>
+      </c>
+      <c r="E34">
+        <v>33</v>
+      </c>
+      <c r="F34">
+        <v>0.6470588235294118</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>1474</v>
+      </c>
+      <c r="C35">
+        <v>42.5</v>
+      </c>
+      <c r="D35">
+        <v>51</v>
+      </c>
+      <c r="E35">
+        <v>34</v>
+      </c>
+      <c r="F35">
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>16</v>
+      </c>
+      <c r="B36">
+        <v>22</v>
+      </c>
+      <c r="C36">
+        <v>42</v>
+      </c>
+      <c r="D36">
+        <v>50</v>
+      </c>
+      <c r="E36">
+        <v>34</v>
+      </c>
+      <c r="F36">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>15</v>
+      </c>
+      <c r="B37">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>41.5</v>
+      </c>
+      <c r="D37">
+        <v>49</v>
+      </c>
+      <c r="E37">
+        <v>34</v>
+      </c>
+      <c r="F37">
+        <v>0.69387755102040816</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>14</v>
+      </c>
+      <c r="B38">
+        <v>57</v>
+      </c>
+      <c r="C38">
+        <v>41</v>
+      </c>
+      <c r="D38">
+        <v>48</v>
+      </c>
+      <c r="E38">
+        <v>34</v>
+      </c>
+      <c r="F38">
+        <v>0.70833333333333337</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>13</v>
+      </c>
+      <c r="B39">
+        <v>5</v>
+      </c>
+      <c r="C39">
+        <v>40.5</v>
+      </c>
+      <c r="D39">
+        <v>47</v>
+      </c>
+      <c r="E39">
+        <v>34</v>
+      </c>
+      <c r="F39">
+        <v>0.72340425531914898</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>12</v>
+      </c>
+      <c r="B40">
+        <v>1890</v>
+      </c>
+      <c r="C40">
+        <v>40</v>
+      </c>
+      <c r="D40">
+        <v>46</v>
+      </c>
+      <c r="E40">
+        <v>34</v>
+      </c>
+      <c r="F40">
+        <v>0.73913043478260865</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>11</v>
+      </c>
+      <c r="B41">
+        <v>13</v>
+      </c>
+      <c r="C41">
+        <v>39.5</v>
+      </c>
+      <c r="D41">
+        <v>45</v>
+      </c>
+      <c r="E41">
+        <v>34</v>
+      </c>
+      <c r="F41">
+        <v>0.75555555555555554</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>10</v>
+      </c>
+      <c r="B42">
+        <v>132</v>
+      </c>
+      <c r="C42">
+        <v>39</v>
+      </c>
+      <c r="D42">
+        <v>44</v>
+      </c>
+      <c r="E42">
+        <v>34</v>
+      </c>
+      <c r="F42">
+        <v>0.77272727272727271</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>9</v>
+      </c>
+      <c r="B43">
+        <v>318</v>
+      </c>
+      <c r="C43">
+        <v>39.5</v>
+      </c>
+      <c r="D43">
+        <v>44</v>
+      </c>
+      <c r="E43">
+        <v>35</v>
+      </c>
+      <c r="F43">
+        <v>0.79545454545454541</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>8</v>
+      </c>
+      <c r="B44">
+        <v>871</v>
+      </c>
+      <c r="C44">
+        <v>40</v>
+      </c>
+      <c r="D44">
+        <v>44</v>
+      </c>
+      <c r="E44">
+        <v>36</v>
+      </c>
+      <c r="F44">
+        <v>0.81818181818181823</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>7</v>
+      </c>
+      <c r="B45">
+        <v>2</v>
+      </c>
+      <c r="C45">
+        <v>39.5</v>
+      </c>
+      <c r="D45">
+        <v>43</v>
+      </c>
+      <c r="E45">
+        <v>36</v>
+      </c>
+      <c r="F45">
+        <v>0.83720930232558144</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>6</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>39</v>
+      </c>
+      <c r="D46">
+        <v>42</v>
+      </c>
+      <c r="E46">
+        <v>36</v>
+      </c>
+      <c r="F46">
+        <v>0.8571428571428571</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>